<commit_message>
Added Advanced Search and PO PDF Report Validations
</commit_message>
<xml_diff>
--- a/LMG_PLM/src/test/resources/testdata.xlsx
+++ b/LMG_PLM/src/test/resources/testdata.xlsx
@@ -14,8 +14,10 @@
   <sheets>
     <sheet name="Login_Cred_PLM" sheetId="1" r:id="rId1"/>
     <sheet name="Create_Tech_Spec" sheetId="2" r:id="rId2"/>
-    <sheet name="Data" sheetId="4" r:id="rId3"/>
-    <sheet name="Dropdown_Options" sheetId="3" r:id="rId4"/>
+    <sheet name="Create_Tech_Spec_Multiple" sheetId="6" r:id="rId3"/>
+    <sheet name="AdvanceSearch_Tech_Spec" sheetId="5" r:id="rId4"/>
+    <sheet name="Data" sheetId="4" r:id="rId5"/>
+    <sheet name="Dropdown_Options" sheetId="3" r:id="rId6"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -27,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="365" uniqueCount="184">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="618" uniqueCount="232">
   <si>
     <t>UserName</t>
   </si>
@@ -569,23 +571,167 @@
     <t>50</t>
   </si>
   <si>
-    <t>21/11/2023</t>
-  </si>
-  <si>
-    <t>21/12/2023</t>
-  </si>
-  <si>
     <t>Number of Rows to search-17</t>
   </si>
   <si>
     <t>End</t>
+  </si>
+  <si>
+    <t>048 TB24JUL23-2 TESTING</t>
+  </si>
+  <si>
+    <t>UpperCase</t>
+  </si>
+  <si>
+    <t>CARRY ALL COSMETICS</t>
+  </si>
+  <si>
+    <t>Item Name</t>
+  </si>
+  <si>
+    <t>Product Category</t>
+  </si>
+  <si>
+    <t>Type of Fit</t>
+  </si>
+  <si>
+    <t>Storyline</t>
+  </si>
+  <si>
+    <t>Hit</t>
+  </si>
+  <si>
+    <t>Buy Program</t>
+  </si>
+  <si>
+    <t>Supplier</t>
+  </si>
+  <si>
+    <t>Dept</t>
+  </si>
+  <si>
+    <t>Dept Desc</t>
+  </si>
+  <si>
+    <t>Group</t>
+  </si>
+  <si>
+    <t>Designer</t>
+  </si>
+  <si>
+    <t>Graphic Designer</t>
+  </si>
+  <si>
+    <t>2PC TSHIRT &amp; DUNGAREE</t>
+  </si>
+  <si>
+    <t>AUTUMN VIBES</t>
+  </si>
+  <si>
+    <t>PROTO</t>
+  </si>
+  <si>
+    <t>TOYS BOYS &amp; GIRLS</t>
+  </si>
+  <si>
+    <t>5636</t>
+  </si>
+  <si>
+    <t>KIMBERLY NETTO</t>
+  </si>
+  <si>
+    <t>NEW</t>
+  </si>
+  <si>
+    <t>NIKITA JAIN</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>60</t>
+  </si>
+  <si>
+    <t>dd/mm/yyyy-Days to add for present date</t>
+  </si>
+  <si>
+    <t>Multiple Styles to be added</t>
+  </si>
+  <si>
+    <t>Value to enter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">All Input Fields </t>
+  </si>
+  <si>
+    <t xml:space="preserve">All Dropdown Main Label Names </t>
+  </si>
+  <si>
+    <t>Dropdown Sub Label Names</t>
+  </si>
+  <si>
+    <t>Value to select</t>
+  </si>
+  <si>
+    <t>Input Fields For Tech Spec</t>
+  </si>
+  <si>
+    <t>Search Icon Label Name-Season</t>
+  </si>
+  <si>
+    <t>Popup Label Name</t>
+  </si>
+  <si>
+    <t>Search Icon Label Name-SubClass</t>
+  </si>
+  <si>
+    <t>Search Icon Label Name-POType</t>
+  </si>
+  <si>
+    <t>Search Icon Label Name-Assortment</t>
+  </si>
+  <si>
+    <t>Search Icon Label Name-BrandUDA</t>
+  </si>
+  <si>
+    <t>Search Icon Label Name-AllBrand(Sub-Brand)</t>
+  </si>
+  <si>
+    <t>Search Icon Label Name-Buyer</t>
+  </si>
+  <si>
+    <t>Search Icon Label Name-Supplier</t>
+  </si>
+  <si>
+    <t>Supplier-Supplier</t>
+  </si>
+  <si>
+    <t>Locator ID Attribute</t>
+  </si>
+  <si>
+    <t>8_@14200_@2_@0_@0_@-1</t>
+  </si>
+  <si>
+    <t>18_@100_@81_@0_@0_@0</t>
+  </si>
+  <si>
+    <t>Size Range</t>
+  </si>
+  <si>
+    <t>Search Icon Label Name-Color Info Name</t>
+  </si>
+  <si>
+    <t>Search Icon Label Name-Color Info Family Shade</t>
+  </si>
+  <si>
+    <t>49 TB24JUL23-2 Testing</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -612,6 +758,26 @@
     <font>
       <b/>
       <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -679,7 +845,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -726,11 +892,51 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -751,7 +957,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -769,8 +974,25 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="6" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1052,7 +1274,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1073,13 +1295,16 @@
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="33" t="s">
         <v>3</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -1087,8 +1312,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:CC9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AX1" workbookViewId="0">
-      <selection activeCell="BE4" sqref="BE4"/>
+    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
+      <selection activeCell="R5" sqref="R5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1227,26 +1452,26 @@
       <c r="V1" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="X1" s="17" t="s">
+      <c r="X1" s="16" t="s">
         <v>142</v>
       </c>
-      <c r="Y1" s="21" t="s">
+      <c r="Y1" s="20" t="s">
         <v>145</v>
       </c>
-      <c r="AA1" s="17" t="s">
+      <c r="AA1" s="16" t="s">
         <v>109</v>
       </c>
-      <c r="AY1" s="17" t="s">
+      <c r="AY1" s="16" t="s">
         <v>110</v>
       </c>
-      <c r="BH1" s="17" t="s">
+      <c r="BH1" s="16" t="s">
         <v>122</v>
       </c>
       <c r="BT1" s="6" t="s">
         <v>164</v>
       </c>
       <c r="CC1" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="2" spans="1:81" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1272,10 +1497,10 @@
       </c>
       <c r="I2" s="15"/>
       <c r="J2" s="15" t="s">
-        <v>60</v>
+        <v>207</v>
       </c>
       <c r="K2" s="15" t="s">
-        <v>60</v>
+        <v>207</v>
       </c>
       <c r="L2" s="10" t="s">
         <v>29</v>
@@ -1310,164 +1535,164 @@
       <c r="V2" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="X2" s="21" t="s">
+      <c r="X2" s="20" t="s">
         <v>143</v>
       </c>
-      <c r="Y2" s="21" t="s">
+      <c r="Y2" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="AA2" s="17" t="s">
+      <c r="AA2" s="16" t="s">
         <v>107</v>
       </c>
-      <c r="AB2" s="18" t="s">
+      <c r="AB2" s="17" t="s">
         <v>67</v>
       </c>
-      <c r="AC2" s="18" t="s">
+      <c r="AC2" s="17" t="s">
         <v>68</v>
       </c>
-      <c r="AD2" s="18" t="s">
+      <c r="AD2" s="17" t="s">
         <v>71</v>
       </c>
-      <c r="AE2" s="18" t="s">
+      <c r="AE2" s="17" t="s">
         <v>72</v>
       </c>
-      <c r="AF2" s="18" t="s">
+      <c r="AF2" s="17" t="s">
         <v>73</v>
       </c>
-      <c r="AG2" s="18" t="s">
+      <c r="AG2" s="17" t="s">
         <v>74</v>
       </c>
-      <c r="AH2" s="18" t="s">
+      <c r="AH2" s="17" t="s">
         <v>75</v>
       </c>
-      <c r="AI2" s="18" t="s">
+      <c r="AI2" s="17" t="s">
         <v>76</v>
       </c>
-      <c r="AJ2" s="18" t="s">
+      <c r="AJ2" s="17" t="s">
         <v>77</v>
       </c>
-      <c r="AK2" s="18" t="s">
+      <c r="AK2" s="17" t="s">
         <v>78</v>
       </c>
-      <c r="AL2" s="18" t="s">
+      <c r="AL2" s="17" t="s">
         <v>79</v>
       </c>
-      <c r="AM2" s="18" t="s">
+      <c r="AM2" s="17" t="s">
         <v>80</v>
       </c>
-      <c r="AN2" s="18" t="s">
+      <c r="AN2" s="17" t="s">
         <v>81</v>
       </c>
-      <c r="AO2" s="18" t="s">
+      <c r="AO2" s="17" t="s">
         <v>82</v>
       </c>
-      <c r="AP2" s="18" t="s">
+      <c r="AP2" s="17" t="s">
         <v>83</v>
       </c>
-      <c r="AQ2" s="18" t="s">
+      <c r="AQ2" s="17" t="s">
         <v>84</v>
       </c>
-      <c r="AR2" s="18" t="s">
+      <c r="AR2" s="17" t="s">
         <v>85</v>
       </c>
-      <c r="AS2" s="18" t="s">
+      <c r="AS2" s="17" t="s">
         <v>86</v>
       </c>
-      <c r="AT2" s="18" t="s">
+      <c r="AT2" s="17" t="s">
         <v>87</v>
       </c>
-      <c r="AU2" s="18" t="s">
+      <c r="AU2" s="17" t="s">
         <v>88</v>
       </c>
-      <c r="AV2" s="18" t="s">
+      <c r="AV2" s="17" t="s">
         <v>89</v>
       </c>
-      <c r="AW2" s="18" t="s">
+      <c r="AW2" s="17" t="s">
         <v>90</v>
       </c>
-      <c r="AY2" s="17" t="s">
+      <c r="AY2" s="16" t="s">
         <v>107</v>
       </c>
-      <c r="AZ2" s="19" t="s">
+      <c r="AZ2" s="18" t="s">
         <v>111</v>
       </c>
-      <c r="BA2" s="19" t="s">
+      <c r="BA2" s="18" t="s">
         <v>112</v>
       </c>
-      <c r="BB2" s="19" t="s">
+      <c r="BB2" s="18" t="s">
         <v>113</v>
       </c>
-      <c r="BC2" s="19" t="s">
+      <c r="BC2" s="18" t="s">
         <v>114</v>
       </c>
-      <c r="BD2" s="19" t="s">
+      <c r="BD2" s="18" t="s">
         <v>115</v>
       </c>
-      <c r="BE2" s="19" t="s">
+      <c r="BE2" s="18" t="s">
         <v>116</v>
       </c>
-      <c r="BF2" s="19" t="s">
+      <c r="BF2" s="18" t="s">
         <v>117</v>
       </c>
-      <c r="BH2" s="17" t="s">
+      <c r="BH2" s="16" t="s">
         <v>107</v>
       </c>
-      <c r="BI2" s="20" t="s">
+      <c r="BI2" s="19" t="s">
         <v>123</v>
       </c>
-      <c r="BJ2" s="20" t="s">
+      <c r="BJ2" s="19" t="s">
         <v>124</v>
       </c>
-      <c r="BK2" s="20" t="s">
+      <c r="BK2" s="19" t="s">
         <v>125</v>
       </c>
-      <c r="BL2" s="20" t="s">
+      <c r="BL2" s="19" t="s">
         <v>126</v>
       </c>
-      <c r="BM2" s="20" t="s">
+      <c r="BM2" s="19" t="s">
         <v>127</v>
       </c>
-      <c r="BN2" s="20" t="s">
+      <c r="BN2" s="19" t="s">
         <v>128</v>
       </c>
-      <c r="BO2" s="20" t="s">
+      <c r="BO2" s="19" t="s">
         <v>129</v>
       </c>
-      <c r="BP2" s="20" t="s">
+      <c r="BP2" s="19" t="s">
         <v>130</v>
       </c>
-      <c r="BQ2" s="20" t="s">
+      <c r="BQ2" s="19" t="s">
         <v>131</v>
       </c>
-      <c r="BR2" s="20" t="s">
+      <c r="BR2" s="19" t="s">
         <v>132</v>
       </c>
-      <c r="BT2" s="17" t="s">
+      <c r="BT2" s="16" t="s">
         <v>165</v>
       </c>
-      <c r="BU2" s="27" t="s">
+      <c r="BU2" s="26" t="s">
         <v>167</v>
       </c>
-      <c r="BV2" s="27" t="s">
+      <c r="BV2" s="26" t="s">
         <v>168</v>
       </c>
-      <c r="BW2" s="27" t="s">
+      <c r="BW2" s="26" t="s">
         <v>169</v>
       </c>
-      <c r="BX2" s="27" t="s">
+      <c r="BX2" s="26" t="s">
         <v>170</v>
       </c>
-      <c r="BY2" s="27" t="s">
+      <c r="BY2" s="26" t="s">
         <v>171</v>
       </c>
-      <c r="BZ2" s="27" t="s">
+      <c r="BZ2" s="26" t="s">
         <v>172</v>
       </c>
-      <c r="CA2" s="27" t="s">
+      <c r="CA2" s="26" t="s">
         <v>173</v>
       </c>
       <c r="CC2" s="8" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="3" spans="1:81" ht="33" customHeight="1" x14ac:dyDescent="0.25">
@@ -1499,10 +1724,10 @@
         <v>45</v>
       </c>
       <c r="J3" s="13" t="s">
-        <v>180</v>
+        <v>205</v>
       </c>
       <c r="K3" s="13" t="s">
-        <v>181</v>
+        <v>206</v>
       </c>
       <c r="L3" s="9" t="s">
         <v>46</v>
@@ -1543,7 +1768,7 @@
       <c r="Y3" s="9" t="s">
         <v>160</v>
       </c>
-      <c r="AA3" s="17" t="s">
+      <c r="AA3" s="16" t="s">
         <v>108</v>
       </c>
       <c r="AB3" s="7" t="s">
@@ -1612,7 +1837,7 @@
       <c r="AW3" s="9" t="s">
         <v>105</v>
       </c>
-      <c r="AY3" s="17" t="s">
+      <c r="AY3" s="16" t="s">
         <v>108</v>
       </c>
       <c r="AZ3" s="9" t="s">
@@ -1636,7 +1861,7 @@
       <c r="BF3" s="9" t="s">
         <v>119</v>
       </c>
-      <c r="BH3" s="17" t="s">
+      <c r="BH3" s="16" t="s">
         <v>108</v>
       </c>
       <c r="BI3" s="11" t="s">
@@ -1667,7 +1892,7 @@
         <v>140</v>
       </c>
       <c r="BR3" s="9"/>
-      <c r="BT3" s="17" t="s">
+      <c r="BT3" s="16" t="s">
         <v>166</v>
       </c>
       <c r="BU3" s="11" t="s">
@@ -1679,38 +1904,38 @@
       <c r="BW3" s="11" t="s">
         <v>176</v>
       </c>
-      <c r="BX3" s="26" t="s">
+      <c r="BX3" s="25" t="s">
         <v>177</v>
       </c>
-      <c r="BY3" s="26" t="s">
+      <c r="BY3" s="25" t="s">
         <v>178</v>
       </c>
-      <c r="BZ3" s="26" t="s">
+      <c r="BZ3" s="25" t="s">
         <v>177</v>
       </c>
-      <c r="CA3" s="26" t="s">
+      <c r="CA3" s="25" t="s">
         <v>179</v>
       </c>
       <c r="CC3" s="8" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="4" spans="1:81" ht="45" x14ac:dyDescent="0.25">
-      <c r="J4" s="16"/>
-      <c r="AA4" s="17" t="s">
+      <c r="J4" s="32"/>
+      <c r="AA4" s="16" t="s">
         <v>163</v>
       </c>
-      <c r="AY4" s="17" t="s">
+      <c r="AY4" s="16" t="s">
         <v>161</v>
       </c>
-      <c r="BH4" s="17" t="s">
+      <c r="BH4" s="16" t="s">
         <v>162</v>
       </c>
-      <c r="BT4" s="17" t="s">
-        <v>182</v>
+      <c r="BT4" s="16" t="s">
+        <v>180</v>
       </c>
       <c r="CC4" s="8" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="9" spans="1:81" x14ac:dyDescent="0.25">
@@ -1723,6 +1948,1108 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:CU13"/>
+  <sheetViews>
+    <sheetView topLeftCell="S1" workbookViewId="0">
+      <selection activeCell="V13" sqref="V13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="32.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="4" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="30.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="31" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="17" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="31" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="33.5703125" bestFit="1" customWidth="1"/>
+    <col min="21" max="22" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="32.42578125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="41.7109375" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="28.28515625" bestFit="1" customWidth="1"/>
+    <col min="30" max="31" width="15" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="45.140625" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="23.140625" style="8" customWidth="1"/>
+    <col min="35" max="35" width="52.28515625" style="8" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="31.140625" style="8" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="30.7109375" style="8" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="24" style="8" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="30.7109375" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="26.5703125" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="25.85546875" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="31" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="7" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="10" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="5" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="57" max="57" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="58" max="58" width="24.5703125" bestFit="1" customWidth="1"/>
+    <col min="59" max="59" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="61" max="61" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="62" max="62" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="63" max="63" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="66" max="66" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="67" max="67" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="68" max="68" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="69" max="70" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="71" max="71" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="72" max="72" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="73" max="73" width="32.85546875" bestFit="1" customWidth="1"/>
+    <col min="74" max="74" width="8" bestFit="1" customWidth="1"/>
+    <col min="75" max="75" width="5.28515625" bestFit="1" customWidth="1"/>
+    <col min="77" max="77" width="30.140625" bestFit="1" customWidth="1"/>
+    <col min="78" max="78" width="5.42578125" bestFit="1" customWidth="1"/>
+    <col min="79" max="79" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="80" max="80" width="5.42578125" bestFit="1" customWidth="1"/>
+    <col min="81" max="81" width="4.85546875" bestFit="1" customWidth="1"/>
+    <col min="82" max="82" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="83" max="83" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="84" max="84" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="86" max="86" width="4.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:99" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
+        <v>210</v>
+      </c>
+      <c r="B1" s="38"/>
+      <c r="C1" s="38"/>
+      <c r="D1" s="34" t="s">
+        <v>207</v>
+      </c>
+      <c r="E1" s="34" t="s">
+        <v>207</v>
+      </c>
+      <c r="F1" s="10" t="s">
+        <v>191</v>
+      </c>
+      <c r="G1" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="I1" s="6" t="s">
+        <v>215</v>
+      </c>
+      <c r="J1" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="L1" s="6" t="s">
+        <v>217</v>
+      </c>
+      <c r="M1" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="N1" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="O1" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="Q1" s="6" t="s">
+        <v>218</v>
+      </c>
+      <c r="R1" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="T1" s="6" t="s">
+        <v>219</v>
+      </c>
+      <c r="U1" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="W1" s="6" t="s">
+        <v>220</v>
+      </c>
+      <c r="X1" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="Z1" s="6" t="s">
+        <v>221</v>
+      </c>
+      <c r="AA1" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="AC1" s="6" t="s">
+        <v>222</v>
+      </c>
+      <c r="AD1" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="AF1" s="6" t="s">
+        <v>229</v>
+      </c>
+      <c r="AG1" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="AH1"/>
+      <c r="AI1" s="6" t="s">
+        <v>230</v>
+      </c>
+      <c r="AJ1" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="AL1" s="6" t="s">
+        <v>223</v>
+      </c>
+      <c r="AM1" s="12" t="s">
+        <v>224</v>
+      </c>
+      <c r="AO1" s="6" t="s">
+        <v>211</v>
+      </c>
+      <c r="AP1" s="12" t="s">
+        <v>64</v>
+      </c>
+      <c r="AQ1" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="AS1" s="16" t="s">
+        <v>109</v>
+      </c>
+      <c r="AT1" s="8"/>
+      <c r="AU1" s="8"/>
+      <c r="AV1" s="8"/>
+      <c r="AW1" s="8"/>
+      <c r="AX1" s="8"/>
+      <c r="AY1" s="8"/>
+      <c r="AZ1" s="8"/>
+      <c r="BA1" s="8"/>
+      <c r="BB1" s="8"/>
+      <c r="BC1" s="8"/>
+      <c r="BD1" s="8"/>
+      <c r="BE1" s="8"/>
+      <c r="BF1" s="8"/>
+      <c r="BG1" s="8"/>
+      <c r="BH1" s="8"/>
+      <c r="BI1" s="8"/>
+      <c r="BJ1" s="8"/>
+      <c r="BK1" s="8"/>
+      <c r="BL1" s="8"/>
+      <c r="BM1" s="8"/>
+      <c r="BN1" s="8"/>
+      <c r="BO1" s="8"/>
+      <c r="BP1" s="8"/>
+      <c r="BQ1" s="16" t="s">
+        <v>110</v>
+      </c>
+      <c r="BR1" s="8"/>
+      <c r="BS1" s="8"/>
+      <c r="BT1" s="8"/>
+      <c r="BU1" s="8"/>
+      <c r="BV1" s="8"/>
+      <c r="BW1" s="8"/>
+      <c r="BX1" s="8"/>
+      <c r="BY1" s="8"/>
+      <c r="BZ1" s="16" t="s">
+        <v>122</v>
+      </c>
+      <c r="CA1" s="8"/>
+      <c r="CB1" s="8"/>
+      <c r="CC1" s="8"/>
+      <c r="CD1" s="8"/>
+      <c r="CE1" s="8"/>
+      <c r="CF1" s="8"/>
+      <c r="CG1" s="8"/>
+      <c r="CH1" s="8"/>
+      <c r="CI1" s="8"/>
+      <c r="CJ1" s="8"/>
+      <c r="CK1" s="8"/>
+      <c r="CL1" s="6" t="s">
+        <v>164</v>
+      </c>
+      <c r="CM1" s="8"/>
+      <c r="CN1" s="8"/>
+      <c r="CO1" s="8"/>
+      <c r="CP1" s="8"/>
+      <c r="CQ1" s="8"/>
+      <c r="CR1" s="8"/>
+      <c r="CS1" s="8"/>
+      <c r="CT1" s="8"/>
+      <c r="CU1" s="8" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="2" spans="1:99" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>214</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="D2" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="E2" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="F2" s="37" t="s">
+        <v>66</v>
+      </c>
+      <c r="G2" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="I2" s="6" t="s">
+        <v>216</v>
+      </c>
+      <c r="J2" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="L2" s="6" t="s">
+        <v>216</v>
+      </c>
+      <c r="M2" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="N2" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="O2" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q2" s="6" t="s">
+        <v>216</v>
+      </c>
+      <c r="R2" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="T2" s="6" t="s">
+        <v>216</v>
+      </c>
+      <c r="U2" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="W2" s="6" t="s">
+        <v>216</v>
+      </c>
+      <c r="X2" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="Z2" s="6" t="s">
+        <v>216</v>
+      </c>
+      <c r="AA2" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="AC2" s="6" t="s">
+        <v>216</v>
+      </c>
+      <c r="AD2" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="AF2" s="6" t="s">
+        <v>216</v>
+      </c>
+      <c r="AG2" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="AH2"/>
+      <c r="AI2" s="6" t="s">
+        <v>216</v>
+      </c>
+      <c r="AJ2" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="AL2" s="6" t="s">
+        <v>216</v>
+      </c>
+      <c r="AM2" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="AO2" s="6" t="s">
+        <v>212</v>
+      </c>
+      <c r="AP2" s="12" t="s">
+        <v>228</v>
+      </c>
+      <c r="AQ2" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="AS2" s="16" t="s">
+        <v>107</v>
+      </c>
+      <c r="AT2" s="17" t="s">
+        <v>67</v>
+      </c>
+      <c r="AU2" s="17" t="s">
+        <v>68</v>
+      </c>
+      <c r="AV2" s="17" t="s">
+        <v>71</v>
+      </c>
+      <c r="AW2" s="17" t="s">
+        <v>72</v>
+      </c>
+      <c r="AX2" s="17" t="s">
+        <v>73</v>
+      </c>
+      <c r="AY2" s="17" t="s">
+        <v>74</v>
+      </c>
+      <c r="AZ2" s="17" t="s">
+        <v>75</v>
+      </c>
+      <c r="BA2" s="17" t="s">
+        <v>76</v>
+      </c>
+      <c r="BB2" s="17" t="s">
+        <v>77</v>
+      </c>
+      <c r="BC2" s="17" t="s">
+        <v>78</v>
+      </c>
+      <c r="BD2" s="17" t="s">
+        <v>79</v>
+      </c>
+      <c r="BE2" s="17" t="s">
+        <v>80</v>
+      </c>
+      <c r="BF2" s="17" t="s">
+        <v>81</v>
+      </c>
+      <c r="BG2" s="17" t="s">
+        <v>82</v>
+      </c>
+      <c r="BH2" s="17" t="s">
+        <v>83</v>
+      </c>
+      <c r="BI2" s="17" t="s">
+        <v>84</v>
+      </c>
+      <c r="BJ2" s="17" t="s">
+        <v>85</v>
+      </c>
+      <c r="BK2" s="17" t="s">
+        <v>86</v>
+      </c>
+      <c r="BL2" s="17" t="s">
+        <v>87</v>
+      </c>
+      <c r="BM2" s="17" t="s">
+        <v>88</v>
+      </c>
+      <c r="BN2" s="17" t="s">
+        <v>89</v>
+      </c>
+      <c r="BO2" s="17" t="s">
+        <v>90</v>
+      </c>
+      <c r="BP2" s="8"/>
+      <c r="BQ2" s="16" t="s">
+        <v>107</v>
+      </c>
+      <c r="BR2" s="18" t="s">
+        <v>111</v>
+      </c>
+      <c r="BS2" s="18" t="s">
+        <v>112</v>
+      </c>
+      <c r="BT2" s="18" t="s">
+        <v>113</v>
+      </c>
+      <c r="BU2" s="18" t="s">
+        <v>114</v>
+      </c>
+      <c r="BV2" s="18" t="s">
+        <v>115</v>
+      </c>
+      <c r="BW2" s="18" t="s">
+        <v>116</v>
+      </c>
+      <c r="BX2" s="18" t="s">
+        <v>117</v>
+      </c>
+      <c r="BY2" s="8"/>
+      <c r="BZ2" s="16" t="s">
+        <v>107</v>
+      </c>
+      <c r="CA2" s="19" t="s">
+        <v>123</v>
+      </c>
+      <c r="CB2" s="19" t="s">
+        <v>124</v>
+      </c>
+      <c r="CC2" s="19" t="s">
+        <v>125</v>
+      </c>
+      <c r="CD2" s="19" t="s">
+        <v>126</v>
+      </c>
+      <c r="CE2" s="19" t="s">
+        <v>127</v>
+      </c>
+      <c r="CF2" s="19" t="s">
+        <v>128</v>
+      </c>
+      <c r="CG2" s="19" t="s">
+        <v>129</v>
+      </c>
+      <c r="CH2" s="19" t="s">
+        <v>130</v>
+      </c>
+      <c r="CI2" s="19" t="s">
+        <v>131</v>
+      </c>
+      <c r="CJ2" s="19" t="s">
+        <v>132</v>
+      </c>
+      <c r="CK2" s="8"/>
+      <c r="CL2" s="16" t="s">
+        <v>165</v>
+      </c>
+      <c r="CM2" s="26" t="s">
+        <v>167</v>
+      </c>
+      <c r="CN2" s="26" t="s">
+        <v>168</v>
+      </c>
+      <c r="CO2" s="26" t="s">
+        <v>169</v>
+      </c>
+      <c r="CP2" s="26" t="s">
+        <v>170</v>
+      </c>
+      <c r="CQ2" s="26" t="s">
+        <v>171</v>
+      </c>
+      <c r="CR2" s="26" t="s">
+        <v>172</v>
+      </c>
+      <c r="CS2" s="26" t="s">
+        <v>173</v>
+      </c>
+      <c r="CT2" s="8"/>
+      <c r="CU2" s="8" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="3" spans="1:99" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
+        <v>209</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="D3" s="13" t="s">
+        <v>205</v>
+      </c>
+      <c r="E3" s="35" t="s">
+        <v>206</v>
+      </c>
+      <c r="F3" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="G3" s="36" t="s">
+        <v>50</v>
+      </c>
+      <c r="I3" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="J3" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="L3" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="M3" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="N3" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="O3" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q3" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="R3" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="T3" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="U3" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="W3" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="X3" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="Z3" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="AA3" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="AC3" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="AD3" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="AF3" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="AG3" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="AH3"/>
+      <c r="AI3" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="AJ3" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="AL3" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="AM3" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="AO3" s="6" t="s">
+        <v>213</v>
+      </c>
+      <c r="AP3" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="AQ3" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="AS3" s="16" t="s">
+        <v>108</v>
+      </c>
+      <c r="AT3" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="AU3" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="AV3" s="9" t="s">
+        <v>141</v>
+      </c>
+      <c r="AW3" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="AX3" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="AY3" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="AZ3" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="BA3" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="BB3" s="9" t="s">
+        <v>95</v>
+      </c>
+      <c r="BC3" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="BD3" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="BE3" s="9" t="s">
+        <v>96</v>
+      </c>
+      <c r="BF3" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="BG3" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="BH3" s="9" t="s">
+        <v>99</v>
+      </c>
+      <c r="BI3" s="9" t="s">
+        <v>100</v>
+      </c>
+      <c r="BJ3" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="BK3" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="BL3" s="11" t="s">
+        <v>106</v>
+      </c>
+      <c r="BM3" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="BN3" s="9" t="s">
+        <v>104</v>
+      </c>
+      <c r="BO3" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="BP3" s="8"/>
+      <c r="BQ3" s="16" t="s">
+        <v>108</v>
+      </c>
+      <c r="BR3" s="9" t="s">
+        <v>104</v>
+      </c>
+      <c r="BS3" s="11" t="s">
+        <v>120</v>
+      </c>
+      <c r="BT3" s="9" t="s">
+        <v>118</v>
+      </c>
+      <c r="BU3" s="9" t="s">
+        <v>104</v>
+      </c>
+      <c r="BV3" s="11" t="s">
+        <v>121</v>
+      </c>
+      <c r="BW3" s="11" t="s">
+        <v>121</v>
+      </c>
+      <c r="BX3" s="9" t="s">
+        <v>119</v>
+      </c>
+      <c r="BY3" s="8"/>
+      <c r="BZ3" s="16" t="s">
+        <v>108</v>
+      </c>
+      <c r="CA3" s="11" t="s">
+        <v>133</v>
+      </c>
+      <c r="CB3" s="11" t="s">
+        <v>138</v>
+      </c>
+      <c r="CC3" s="9" t="s">
+        <v>134</v>
+      </c>
+      <c r="CD3" s="9" t="s">
+        <v>135</v>
+      </c>
+      <c r="CE3" s="9" t="s">
+        <v>135</v>
+      </c>
+      <c r="CF3" s="9" t="s">
+        <v>136</v>
+      </c>
+      <c r="CG3" s="9" t="s">
+        <v>137</v>
+      </c>
+      <c r="CH3" s="11" t="s">
+        <v>139</v>
+      </c>
+      <c r="CI3" s="11" t="s">
+        <v>140</v>
+      </c>
+      <c r="CJ3" s="9"/>
+      <c r="CK3" s="8"/>
+      <c r="CL3" s="16" t="s">
+        <v>166</v>
+      </c>
+      <c r="CM3" s="11" t="s">
+        <v>174</v>
+      </c>
+      <c r="CN3" s="11" t="s">
+        <v>175</v>
+      </c>
+      <c r="CO3" s="11" t="s">
+        <v>176</v>
+      </c>
+      <c r="CP3" s="25" t="s">
+        <v>177</v>
+      </c>
+      <c r="CQ3" s="25" t="s">
+        <v>178</v>
+      </c>
+      <c r="CR3" s="25" t="s">
+        <v>177</v>
+      </c>
+      <c r="CS3" s="25" t="s">
+        <v>179</v>
+      </c>
+      <c r="CT3" s="8"/>
+      <c r="CU3" s="8" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="4" spans="1:99" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AH4"/>
+      <c r="AI4"/>
+      <c r="AJ4"/>
+      <c r="AL4"/>
+      <c r="AM4"/>
+      <c r="AO4" s="6" t="s">
+        <v>225</v>
+      </c>
+      <c r="AP4" s="11" t="s">
+        <v>226</v>
+      </c>
+      <c r="AQ4" s="11" t="s">
+        <v>227</v>
+      </c>
+      <c r="AS4" s="16" t="s">
+        <v>163</v>
+      </c>
+      <c r="AT4" s="8"/>
+      <c r="AU4" s="8"/>
+      <c r="AV4" s="8"/>
+      <c r="AW4" s="8"/>
+      <c r="AX4" s="8"/>
+      <c r="AY4" s="8"/>
+      <c r="AZ4" s="8"/>
+      <c r="BA4" s="8"/>
+      <c r="BB4" s="8"/>
+      <c r="BC4" s="8"/>
+      <c r="BD4" s="8"/>
+      <c r="BE4" s="8"/>
+      <c r="BF4" s="8"/>
+      <c r="BG4" s="8"/>
+      <c r="BH4" s="8"/>
+      <c r="BI4" s="8"/>
+      <c r="BJ4" s="8"/>
+      <c r="BK4" s="8"/>
+      <c r="BL4" s="8"/>
+      <c r="BM4" s="8"/>
+      <c r="BN4" s="8"/>
+      <c r="BO4" s="8"/>
+      <c r="BP4" s="8"/>
+      <c r="BQ4" s="16" t="s">
+        <v>161</v>
+      </c>
+      <c r="BR4" s="8"/>
+      <c r="BS4" s="8"/>
+      <c r="BT4" s="8"/>
+      <c r="BU4" s="8"/>
+      <c r="BV4" s="8"/>
+      <c r="BW4" s="8"/>
+      <c r="BX4" s="8"/>
+      <c r="BY4" s="8"/>
+      <c r="BZ4" s="16" t="s">
+        <v>162</v>
+      </c>
+      <c r="CA4" s="8"/>
+      <c r="CB4" s="8"/>
+      <c r="CC4" s="8"/>
+      <c r="CD4" s="8"/>
+      <c r="CE4" s="8"/>
+      <c r="CF4" s="8"/>
+      <c r="CG4" s="8"/>
+      <c r="CH4" s="8"/>
+      <c r="CI4" s="8"/>
+      <c r="CJ4" s="8"/>
+      <c r="CK4" s="8"/>
+      <c r="CL4" s="16" t="s">
+        <v>180</v>
+      </c>
+      <c r="CM4" s="8"/>
+      <c r="CN4" s="8"/>
+      <c r="CO4" s="8"/>
+      <c r="CP4" s="8"/>
+      <c r="CQ4" s="8"/>
+      <c r="CR4" s="8"/>
+      <c r="CS4" s="8"/>
+      <c r="CT4" s="8"/>
+      <c r="CU4" s="8" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="5" spans="1:99" x14ac:dyDescent="0.25">
+      <c r="A5" s="6" t="s">
+        <v>208</v>
+      </c>
+      <c r="B5" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="11" t="s">
+        <v>231</v>
+      </c>
+      <c r="AH5"/>
+      <c r="AI5"/>
+      <c r="AJ5"/>
+      <c r="AL5"/>
+      <c r="AM5"/>
+    </row>
+    <row r="6" spans="1:99" x14ac:dyDescent="0.25">
+      <c r="A6" s="8"/>
+      <c r="B6" s="8"/>
+      <c r="AH6"/>
+      <c r="AI6"/>
+      <c r="AJ6"/>
+      <c r="AL6"/>
+      <c r="AM6"/>
+    </row>
+    <row r="7" spans="1:99" x14ac:dyDescent="0.25">
+      <c r="AH7"/>
+      <c r="AI7"/>
+      <c r="AJ7"/>
+      <c r="AL7"/>
+      <c r="AM7"/>
+    </row>
+    <row r="8" spans="1:99" x14ac:dyDescent="0.25">
+      <c r="AH8"/>
+      <c r="AI8"/>
+      <c r="AJ8"/>
+      <c r="AL8"/>
+      <c r="AM8"/>
+    </row>
+    <row r="9" spans="1:99" x14ac:dyDescent="0.25">
+      <c r="AH9"/>
+      <c r="AI9"/>
+      <c r="AJ9"/>
+      <c r="AL9"/>
+      <c r="AM9"/>
+    </row>
+    <row r="10" spans="1:99" x14ac:dyDescent="0.25">
+      <c r="AH10"/>
+      <c r="AI10"/>
+      <c r="AJ10"/>
+      <c r="AL10"/>
+      <c r="AM10"/>
+    </row>
+    <row r="11" spans="1:99" x14ac:dyDescent="0.25">
+      <c r="AH11"/>
+      <c r="AI11"/>
+      <c r="AJ11"/>
+      <c r="AL11"/>
+      <c r="AM11"/>
+    </row>
+    <row r="12" spans="1:99" x14ac:dyDescent="0.25">
+      <c r="AH12"/>
+      <c r="AI12"/>
+      <c r="AJ12"/>
+      <c r="AL12"/>
+      <c r="AM12"/>
+    </row>
+    <row r="13" spans="1:99" x14ac:dyDescent="0.25">
+      <c r="AH13"/>
+      <c r="AI13"/>
+      <c r="AJ13"/>
+      <c r="AL13"/>
+      <c r="AM13"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:S4"/>
+  <sheetViews>
+    <sheetView topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="N3" sqref="N3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" width="23.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="26.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="24" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="15" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="16" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="16.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1" s="27" t="s">
+        <v>22</v>
+      </c>
+      <c r="C1" s="27" t="s">
+        <v>29</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>185</v>
+      </c>
+      <c r="E1" s="27" t="s">
+        <v>33</v>
+      </c>
+      <c r="F1" s="9" t="s">
+        <v>186</v>
+      </c>
+      <c r="G1" s="27" t="s">
+        <v>187</v>
+      </c>
+      <c r="H1" s="9" t="s">
+        <v>188</v>
+      </c>
+      <c r="I1" s="9" t="s">
+        <v>189</v>
+      </c>
+      <c r="J1" s="9" t="s">
+        <v>190</v>
+      </c>
+      <c r="K1" s="27" t="s">
+        <v>191</v>
+      </c>
+      <c r="L1" s="27" t="s">
+        <v>192</v>
+      </c>
+      <c r="M1" s="27" t="s">
+        <v>193</v>
+      </c>
+      <c r="N1" s="27" t="s">
+        <v>145</v>
+      </c>
+      <c r="O1" s="30" t="s">
+        <v>194</v>
+      </c>
+      <c r="P1" s="30" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q1" s="30" t="s">
+        <v>39</v>
+      </c>
+      <c r="R1" s="29" t="s">
+        <v>195</v>
+      </c>
+      <c r="S1" s="9" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="B2" s="27"/>
+      <c r="C2" s="27"/>
+      <c r="D2" s="9"/>
+      <c r="E2" s="27"/>
+      <c r="F2" s="9"/>
+      <c r="G2" s="27"/>
+      <c r="H2" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="I2" s="9"/>
+      <c r="J2" s="9"/>
+      <c r="K2" s="27" t="s">
+        <v>65</v>
+      </c>
+      <c r="L2" s="27"/>
+      <c r="M2" s="27"/>
+      <c r="N2" s="27"/>
+      <c r="O2" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="P2" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q2" s="27"/>
+      <c r="R2" s="9"/>
+      <c r="S2" s="9"/>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" s="28" t="s">
+        <v>182</v>
+      </c>
+      <c r="C3" s="27" t="s">
+        <v>184</v>
+      </c>
+      <c r="D3" s="11" t="s">
+        <v>201</v>
+      </c>
+      <c r="E3" s="27" t="s">
+        <v>45</v>
+      </c>
+      <c r="F3" s="9"/>
+      <c r="G3" s="28" t="s">
+        <v>197</v>
+      </c>
+      <c r="H3" s="9" t="s">
+        <v>198</v>
+      </c>
+      <c r="I3" s="11" t="s">
+        <v>138</v>
+      </c>
+      <c r="J3" s="9"/>
+      <c r="K3" s="27" t="s">
+        <v>53</v>
+      </c>
+      <c r="L3" s="27" t="s">
+        <v>28</v>
+      </c>
+      <c r="M3" s="27"/>
+      <c r="N3" s="27" t="s">
+        <v>199</v>
+      </c>
+      <c r="O3" s="27" t="s">
+        <v>200</v>
+      </c>
+      <c r="P3" s="27" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q3" s="27" t="s">
+        <v>48</v>
+      </c>
+      <c r="R3" s="9" t="s">
+        <v>202</v>
+      </c>
+      <c r="S3" s="9"/>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>183</v>
+      </c>
+      <c r="N4" s="31" t="s">
+        <v>203</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>204</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:CB4"/>
   <sheetViews>
@@ -1811,19 +3138,19 @@
       <c r="A1" s="6" t="s">
         <v>155</v>
       </c>
-      <c r="B1" s="22" t="s">
+      <c r="B1" s="21" t="s">
         <v>147</v>
       </c>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="23"/>
-      <c r="G1" s="22" t="s">
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="G1" s="21" t="s">
         <v>157</v>
       </c>
-      <c r="J1" s="22" t="s">
+      <c r="J1" s="21" t="s">
         <v>153</v>
       </c>
-      <c r="AG1" s="24" t="s">
+      <c r="AG1" s="23" t="s">
         <v>109</v>
       </c>
       <c r="AH1" s="8"/>
@@ -1848,7 +3175,7 @@
       <c r="BA1" s="8"/>
       <c r="BB1" s="8"/>
       <c r="BC1" s="8"/>
-      <c r="BE1" s="24" t="s">
+      <c r="BE1" s="23" t="s">
         <v>110</v>
       </c>
       <c r="BF1" s="8"/>
@@ -1858,7 +3185,7 @@
       <c r="BJ1" s="8"/>
       <c r="BK1" s="8"/>
       <c r="BL1" s="8"/>
-      <c r="BN1" s="24" t="s">
+      <c r="BN1" s="23" t="s">
         <v>122</v>
       </c>
       <c r="BO1" s="8"/>
@@ -1872,7 +3199,7 @@
       <c r="BW1" s="8"/>
       <c r="BX1" s="8"/>
       <c r="BY1" s="8"/>
-      <c r="BZ1" s="24" t="s">
+      <c r="BZ1" s="23" t="s">
         <v>142</v>
       </c>
     </row>
@@ -1961,154 +3288,154 @@
       <c r="AE2" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="AG2" s="17" t="s">
+      <c r="AG2" s="16" t="s">
         <v>107</v>
       </c>
-      <c r="AH2" s="18" t="s">
+      <c r="AH2" s="17" t="s">
         <v>67</v>
       </c>
-      <c r="AI2" s="18" t="s">
+      <c r="AI2" s="17" t="s">
         <v>68</v>
       </c>
-      <c r="AJ2" s="18" t="s">
+      <c r="AJ2" s="17" t="s">
         <v>71</v>
       </c>
-      <c r="AK2" s="18" t="s">
+      <c r="AK2" s="17" t="s">
         <v>72</v>
       </c>
-      <c r="AL2" s="18" t="s">
+      <c r="AL2" s="17" t="s">
         <v>73</v>
       </c>
-      <c r="AM2" s="18" t="s">
+      <c r="AM2" s="17" t="s">
         <v>74</v>
       </c>
-      <c r="AN2" s="18" t="s">
+      <c r="AN2" s="17" t="s">
         <v>75</v>
       </c>
-      <c r="AO2" s="18" t="s">
+      <c r="AO2" s="17" t="s">
         <v>76</v>
       </c>
-      <c r="AP2" s="18" t="s">
+      <c r="AP2" s="17" t="s">
         <v>77</v>
       </c>
-      <c r="AQ2" s="18" t="s">
+      <c r="AQ2" s="17" t="s">
         <v>78</v>
       </c>
-      <c r="AR2" s="18" t="s">
+      <c r="AR2" s="17" t="s">
         <v>79</v>
       </c>
-      <c r="AS2" s="18" t="s">
+      <c r="AS2" s="17" t="s">
         <v>80</v>
       </c>
-      <c r="AT2" s="18" t="s">
+      <c r="AT2" s="17" t="s">
         <v>81</v>
       </c>
-      <c r="AU2" s="18" t="s">
+      <c r="AU2" s="17" t="s">
         <v>82</v>
       </c>
-      <c r="AV2" s="18" t="s">
+      <c r="AV2" s="17" t="s">
         <v>83</v>
       </c>
-      <c r="AW2" s="18" t="s">
+      <c r="AW2" s="17" t="s">
         <v>84</v>
       </c>
-      <c r="AX2" s="18" t="s">
+      <c r="AX2" s="17" t="s">
         <v>85</v>
       </c>
-      <c r="AY2" s="18" t="s">
+      <c r="AY2" s="17" t="s">
         <v>86</v>
       </c>
-      <c r="AZ2" s="18" t="s">
+      <c r="AZ2" s="17" t="s">
         <v>87</v>
       </c>
-      <c r="BA2" s="18" t="s">
+      <c r="BA2" s="17" t="s">
         <v>88</v>
       </c>
-      <c r="BB2" s="18" t="s">
+      <c r="BB2" s="17" t="s">
         <v>89</v>
       </c>
-      <c r="BC2" s="18" t="s">
+      <c r="BC2" s="17" t="s">
         <v>90</v>
       </c>
-      <c r="BE2" s="17" t="s">
+      <c r="BE2" s="16" t="s">
         <v>107</v>
       </c>
-      <c r="BF2" s="19" t="s">
+      <c r="BF2" s="18" t="s">
         <v>111</v>
       </c>
-      <c r="BG2" s="19" t="s">
+      <c r="BG2" s="18" t="s">
         <v>112</v>
       </c>
-      <c r="BH2" s="19" t="s">
+      <c r="BH2" s="18" t="s">
         <v>113</v>
       </c>
-      <c r="BI2" s="19" t="s">
+      <c r="BI2" s="18" t="s">
         <v>114</v>
       </c>
-      <c r="BJ2" s="19" t="s">
+      <c r="BJ2" s="18" t="s">
         <v>115</v>
       </c>
-      <c r="BK2" s="19" t="s">
+      <c r="BK2" s="18" t="s">
         <v>116</v>
       </c>
-      <c r="BL2" s="19" t="s">
+      <c r="BL2" s="18" t="s">
         <v>117</v>
       </c>
-      <c r="BN2" s="17" t="s">
+      <c r="BN2" s="16" t="s">
         <v>107</v>
       </c>
-      <c r="BO2" s="20" t="s">
+      <c r="BO2" s="19" t="s">
         <v>123</v>
       </c>
-      <c r="BP2" s="20" t="s">
+      <c r="BP2" s="19" t="s">
         <v>124</v>
       </c>
-      <c r="BQ2" s="20" t="s">
+      <c r="BQ2" s="19" t="s">
         <v>125</v>
       </c>
-      <c r="BR2" s="20" t="s">
+      <c r="BR2" s="19" t="s">
         <v>126</v>
       </c>
-      <c r="BS2" s="20" t="s">
+      <c r="BS2" s="19" t="s">
         <v>127</v>
       </c>
-      <c r="BT2" s="20" t="s">
+      <c r="BT2" s="19" t="s">
         <v>128</v>
       </c>
-      <c r="BU2" s="20" t="s">
+      <c r="BU2" s="19" t="s">
         <v>129</v>
       </c>
-      <c r="BV2" s="20" t="s">
+      <c r="BV2" s="19" t="s">
         <v>130</v>
       </c>
-      <c r="BW2" s="20" t="s">
+      <c r="BW2" s="19" t="s">
         <v>131</v>
       </c>
-      <c r="BX2" s="20" t="s">
+      <c r="BX2" s="19" t="s">
         <v>132</v>
       </c>
       <c r="BY2" s="8"/>
       <c r="BZ2" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="CA2" s="21" t="s">
+      <c r="CA2" s="20" t="s">
         <v>143</v>
       </c>
-      <c r="CB2" s="21" t="s">
+      <c r="CB2" s="20" t="s">
         <v>145</v>
       </c>
     </row>
     <row r="3" spans="1:80" ht="60" x14ac:dyDescent="0.25">
-      <c r="B3" s="25"/>
-      <c r="C3" s="25"/>
-      <c r="D3" s="25"/>
-      <c r="E3" s="25"/>
-      <c r="H3" s="25"/>
+      <c r="B3" s="24"/>
+      <c r="C3" s="24"/>
+      <c r="D3" s="24"/>
+      <c r="E3" s="24"/>
+      <c r="H3" s="24"/>
       <c r="J3" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="K3" s="23"/>
-      <c r="L3" s="23"/>
+      <c r="K3" s="22"/>
+      <c r="L3" s="22"/>
       <c r="M3" s="10" t="s">
         <v>9</v>
       </c>
@@ -2164,7 +3491,7 @@
       <c r="AE3" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="AG3" s="17" t="s">
+      <c r="AG3" s="16" t="s">
         <v>108</v>
       </c>
       <c r="AH3" s="7" t="s">
@@ -2233,7 +3560,7 @@
       <c r="BC3" s="9" t="s">
         <v>105</v>
       </c>
-      <c r="BE3" s="17" t="s">
+      <c r="BE3" s="16" t="s">
         <v>108</v>
       </c>
       <c r="BF3" s="9" t="s">
@@ -2257,7 +3584,7 @@
       <c r="BL3" s="9" t="s">
         <v>119</v>
       </c>
-      <c r="BN3" s="17" t="s">
+      <c r="BN3" s="16" t="s">
         <v>108</v>
       </c>
       <c r="BO3" s="11" t="s">
@@ -2295,15 +3622,15 @@
       <c r="CA3" s="11" t="s">
         <v>146</v>
       </c>
-      <c r="CB3" s="21" t="s">
+      <c r="CB3" s="20" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:80" x14ac:dyDescent="0.25">
-      <c r="B4" s="25"/>
-      <c r="C4" s="25"/>
-      <c r="D4" s="25"/>
-      <c r="E4" s="25"/>
+      <c r="B4" s="24"/>
+      <c r="C4" s="24"/>
+      <c r="D4" s="24"/>
+      <c r="E4" s="24"/>
       <c r="J4" s="6" t="s">
         <v>151</v>
       </c>
@@ -2386,7 +3713,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A12"/>
   <sheetViews>

</xml_diff>